<commit_message>
created series data tables
</commit_message>
<xml_diff>
--- a/source_data/Qual_5_data.xlsx
+++ b/source_data/Qual_5_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingyan.hu\Downloads\Step2_MinSetStaticCopy_reformat&amp;upload\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gender_data_portal\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21558395-A73C-42E0-ACC7-D392728D740A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77057257-9AFC-474C-AEEC-D68A3CAB6EDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2122,8 +2122,8 @@
   <dimension ref="A1:O316"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A203" sqref="A203:A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11120,6 +11120,9 @@
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>58</v>
+      </c>
       <c r="B192">
         <v>5</v>
       </c>
@@ -11160,7 +11163,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="193" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>58</v>
+      </c>
       <c r="B193">
         <v>5</v>
       </c>
@@ -11201,7 +11207,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="194" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>58</v>
+      </c>
       <c r="B194">
         <v>5</v>
       </c>
@@ -11242,7 +11251,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="195" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>58</v>
+      </c>
       <c r="B195">
         <v>5</v>
       </c>
@@ -11283,7 +11295,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="196" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>58</v>
+      </c>
       <c r="B196">
         <v>5</v>
       </c>
@@ -11324,7 +11339,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="197" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>58</v>
+      </c>
       <c r="B197">
         <v>5</v>
       </c>
@@ -11365,7 +11383,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="198" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>58</v>
+      </c>
       <c r="B198">
         <v>5</v>
       </c>
@@ -11406,7 +11427,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="199" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>58</v>
+      </c>
       <c r="B199">
         <v>5</v>
       </c>
@@ -11447,7 +11471,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="200" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>58</v>
+      </c>
       <c r="B200">
         <v>5</v>
       </c>
@@ -11488,7 +11515,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="201" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>58</v>
+      </c>
       <c r="B201">
         <v>5</v>
       </c>
@@ -11529,7 +11559,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="202" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>58</v>
+      </c>
       <c r="B202">
         <v>5</v>
       </c>
@@ -11570,7 +11603,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="203" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>58</v>
+      </c>
       <c r="B203">
         <v>5</v>
       </c>
@@ -11611,7 +11647,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="204" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>58</v>
+      </c>
       <c r="B204">
         <v>5</v>
       </c>
@@ -11652,7 +11691,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="205" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>58</v>
+      </c>
       <c r="B205">
         <v>5</v>
       </c>
@@ -11693,7 +11735,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="206" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>58</v>
+      </c>
       <c r="B206">
         <v>5</v>
       </c>
@@ -11734,7 +11779,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="207" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>58</v>
+      </c>
       <c r="B207">
         <v>5</v>
       </c>
@@ -11775,7 +11823,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="208" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>58</v>
+      </c>
       <c r="B208">
         <v>5</v>
       </c>
@@ -11816,7 +11867,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="209" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>58</v>
+      </c>
       <c r="B209">
         <v>5</v>
       </c>
@@ -11857,7 +11911,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="210" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>58</v>
+      </c>
       <c r="B210">
         <v>5</v>
       </c>
@@ -11898,7 +11955,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="211" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>58</v>
+      </c>
       <c r="B211">
         <v>5</v>
       </c>
@@ -11939,7 +11999,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="212" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>58</v>
+      </c>
       <c r="B212">
         <v>5</v>
       </c>
@@ -11980,7 +12043,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="213" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>58</v>
+      </c>
       <c r="B213">
         <v>5</v>
       </c>
@@ -12021,7 +12087,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="214" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>58</v>
+      </c>
       <c r="B214">
         <v>5</v>
       </c>
@@ -12062,7 +12131,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="215" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>58</v>
+      </c>
       <c r="B215">
         <v>5</v>
       </c>
@@ -12103,7 +12175,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="216" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>58</v>
+      </c>
       <c r="B216">
         <v>5</v>
       </c>
@@ -12144,7 +12219,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="217" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>58</v>
+      </c>
       <c r="B217">
         <v>5</v>
       </c>
@@ -12185,7 +12263,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="218" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>58</v>
+      </c>
       <c r="B218">
         <v>5</v>
       </c>
@@ -12226,7 +12307,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="219" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>58</v>
+      </c>
       <c r="B219">
         <v>5</v>
       </c>
@@ -12267,7 +12351,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="220" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>58</v>
+      </c>
       <c r="B220">
         <v>5</v>
       </c>
@@ -12308,7 +12395,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="221" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>58</v>
+      </c>
       <c r="B221">
         <v>5</v>
       </c>
@@ -12349,7 +12439,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="222" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>58</v>
+      </c>
       <c r="B222">
         <v>5</v>
       </c>
@@ -12390,7 +12483,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="223" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>58</v>
+      </c>
       <c r="B223">
         <v>5</v>
       </c>
@@ -12431,7 +12527,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="224" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>58</v>
+      </c>
       <c r="B224">
         <v>5</v>
       </c>
@@ -12472,7 +12571,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="225" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>58</v>
+      </c>
       <c r="B225">
         <v>5</v>
       </c>
@@ -12513,7 +12615,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="226" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>58</v>
+      </c>
       <c r="B226">
         <v>5</v>
       </c>
@@ -12554,7 +12659,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="227" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>58</v>
+      </c>
       <c r="B227">
         <v>5</v>
       </c>
@@ -12595,7 +12703,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="228" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>58</v>
+      </c>
       <c r="B228">
         <v>5</v>
       </c>
@@ -12636,7 +12747,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="229" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>58</v>
+      </c>
       <c r="B229">
         <v>5</v>
       </c>
@@ -12677,7 +12791,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="230" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>58</v>
+      </c>
       <c r="B230">
         <v>5</v>
       </c>
@@ -12718,7 +12835,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="231" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>58</v>
+      </c>
       <c r="B231">
         <v>5</v>
       </c>
@@ -12759,7 +12879,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="232" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>58</v>
+      </c>
       <c r="B232">
         <v>5</v>
       </c>
@@ -12800,7 +12923,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="233" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>58</v>
+      </c>
       <c r="B233">
         <v>5</v>
       </c>
@@ -12841,7 +12967,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="234" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>58</v>
+      </c>
       <c r="B234">
         <v>5</v>
       </c>
@@ -12882,7 +13011,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="235" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>58</v>
+      </c>
       <c r="B235">
         <v>5</v>
       </c>
@@ -12923,7 +13055,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="236" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>58</v>
+      </c>
       <c r="B236">
         <v>5</v>
       </c>
@@ -12964,7 +13099,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="237" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>58</v>
+      </c>
       <c r="B237">
         <v>5</v>
       </c>
@@ -13005,7 +13143,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="238" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>58</v>
+      </c>
       <c r="B238">
         <v>5</v>
       </c>
@@ -13046,7 +13187,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="239" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>58</v>
+      </c>
       <c r="B239">
         <v>5</v>
       </c>
@@ -13087,7 +13231,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="240" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>58</v>
+      </c>
       <c r="B240">
         <v>5</v>
       </c>
@@ -13128,7 +13275,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="241" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>58</v>
+      </c>
       <c r="B241">
         <v>5</v>
       </c>
@@ -13169,7 +13319,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="242" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>58</v>
+      </c>
       <c r="B242">
         <v>5</v>
       </c>
@@ -13210,7 +13363,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="243" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>58</v>
+      </c>
       <c r="B243">
         <v>5</v>
       </c>
@@ -13251,7 +13407,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="244" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>58</v>
+      </c>
       <c r="B244">
         <v>5</v>
       </c>
@@ -13292,7 +13451,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="245" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>58</v>
+      </c>
       <c r="B245">
         <v>5</v>
       </c>
@@ -13333,7 +13495,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="246" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>58</v>
+      </c>
       <c r="B246">
         <v>5</v>
       </c>
@@ -13374,7 +13539,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="247" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>58</v>
+      </c>
       <c r="B247">
         <v>5</v>
       </c>
@@ -13415,7 +13583,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="248" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>58</v>
+      </c>
       <c r="B248">
         <v>5</v>
       </c>
@@ -13456,7 +13627,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="249" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>58</v>
+      </c>
       <c r="B249">
         <v>5</v>
       </c>
@@ -13497,7 +13671,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="250" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>58</v>
+      </c>
       <c r="B250">
         <v>5</v>
       </c>
@@ -13538,7 +13715,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="251" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>58</v>
+      </c>
       <c r="B251">
         <v>5</v>
       </c>
@@ -13579,7 +13759,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="252" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>58</v>
+      </c>
       <c r="B252">
         <v>5</v>
       </c>
@@ -13620,7 +13803,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="253" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>58</v>
+      </c>
       <c r="B253">
         <v>5</v>
       </c>
@@ -13661,7 +13847,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="254" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>58</v>
+      </c>
       <c r="B254">
         <v>5</v>
       </c>
@@ -13702,7 +13891,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="255" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>58</v>
+      </c>
       <c r="B255">
         <v>5</v>
       </c>
@@ -13743,7 +13935,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="256" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>58</v>
+      </c>
       <c r="B256">
         <v>5</v>
       </c>
@@ -13784,7 +13979,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="257" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>58</v>
+      </c>
       <c r="B257">
         <v>5</v>
       </c>
@@ -13825,7 +14023,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="258" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>58</v>
+      </c>
       <c r="B258">
         <v>5</v>
       </c>
@@ -13866,7 +14067,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="259" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>58</v>
+      </c>
       <c r="B259">
         <v>5</v>
       </c>
@@ -13907,7 +14111,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="260" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>58</v>
+      </c>
       <c r="B260">
         <v>5</v>
       </c>
@@ -13948,7 +14155,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="261" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>58</v>
+      </c>
       <c r="B261">
         <v>5</v>
       </c>
@@ -13989,7 +14199,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="262" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>58</v>
+      </c>
       <c r="B262">
         <v>5</v>
       </c>
@@ -14030,7 +14243,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="263" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>58</v>
+      </c>
       <c r="B263">
         <v>5</v>
       </c>
@@ -14071,7 +14287,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="264" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>58</v>
+      </c>
       <c r="B264">
         <v>5</v>
       </c>
@@ -14112,7 +14331,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="265" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>58</v>
+      </c>
       <c r="B265">
         <v>5</v>
       </c>
@@ -14153,7 +14375,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="266" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>58</v>
+      </c>
       <c r="B266">
         <v>5</v>
       </c>
@@ -14194,7 +14419,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="267" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>58</v>
+      </c>
       <c r="B267">
         <v>5</v>
       </c>
@@ -14235,7 +14463,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="268" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>58</v>
+      </c>
       <c r="B268">
         <v>5</v>
       </c>
@@ -14276,7 +14507,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="269" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>58</v>
+      </c>
       <c r="B269">
         <v>5</v>
       </c>
@@ -14317,7 +14551,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="270" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>58</v>
+      </c>
       <c r="B270">
         <v>5</v>
       </c>
@@ -14358,7 +14595,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="271" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>58</v>
+      </c>
       <c r="B271">
         <v>5</v>
       </c>
@@ -14399,7 +14639,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="272" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>58</v>
+      </c>
       <c r="B272">
         <v>5</v>
       </c>
@@ -14440,7 +14683,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="273" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>58</v>
+      </c>
       <c r="B273">
         <v>5</v>
       </c>
@@ -14481,7 +14727,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="274" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>58</v>
+      </c>
       <c r="B274">
         <v>5</v>
       </c>
@@ -14522,7 +14771,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="275" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>58</v>
+      </c>
       <c r="B275">
         <v>5</v>
       </c>
@@ -14563,7 +14815,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="276" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>58</v>
+      </c>
       <c r="B276">
         <v>5</v>
       </c>
@@ -14604,7 +14859,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="277" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>58</v>
+      </c>
       <c r="B277">
         <v>5</v>
       </c>
@@ -14645,7 +14903,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="278" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>58</v>
+      </c>
       <c r="B278">
         <v>5</v>
       </c>
@@ -14686,7 +14947,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="279" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>58</v>
+      </c>
       <c r="B279">
         <v>5</v>
       </c>
@@ -14727,7 +14991,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="280" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>58</v>
+      </c>
       <c r="B280">
         <v>5</v>
       </c>
@@ -14768,7 +15035,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="281" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>58</v>
+      </c>
       <c r="B281">
         <v>5</v>
       </c>
@@ -14809,7 +15079,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="282" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>58</v>
+      </c>
       <c r="B282">
         <v>5</v>
       </c>
@@ -14850,7 +15123,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="283" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>58</v>
+      </c>
       <c r="B283">
         <v>5</v>
       </c>
@@ -14891,7 +15167,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="284" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>58</v>
+      </c>
       <c r="B284">
         <v>5</v>
       </c>
@@ -14932,7 +15211,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="285" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>58</v>
+      </c>
       <c r="B285">
         <v>5</v>
       </c>
@@ -14973,7 +15255,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="286" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>58</v>
+      </c>
       <c r="B286">
         <v>5</v>
       </c>
@@ -15014,7 +15299,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="287" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>58</v>
+      </c>
       <c r="B287">
         <v>5</v>
       </c>
@@ -15055,7 +15343,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="288" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>58</v>
+      </c>
       <c r="B288">
         <v>5</v>
       </c>
@@ -15096,7 +15387,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="289" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>58</v>
+      </c>
       <c r="B289">
         <v>5</v>
       </c>
@@ -15137,7 +15431,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="290" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>58</v>
+      </c>
       <c r="B290">
         <v>5</v>
       </c>
@@ -15178,7 +15475,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="291" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>58</v>
+      </c>
       <c r="B291">
         <v>5</v>
       </c>
@@ -15219,7 +15519,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="292" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>58</v>
+      </c>
       <c r="B292">
         <v>5</v>
       </c>
@@ -15260,7 +15563,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="293" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>58</v>
+      </c>
       <c r="B293">
         <v>5</v>
       </c>
@@ -15301,7 +15607,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="294" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>58</v>
+      </c>
       <c r="B294">
         <v>5</v>
       </c>
@@ -15342,7 +15651,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="295" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>58</v>
+      </c>
       <c r="B295">
         <v>5</v>
       </c>
@@ -15383,7 +15695,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="296" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>58</v>
+      </c>
       <c r="B296">
         <v>5</v>
       </c>
@@ -15424,7 +15739,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="297" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>58</v>
+      </c>
       <c r="B297">
         <v>5</v>
       </c>
@@ -15465,7 +15783,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="298" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>58</v>
+      </c>
       <c r="B298">
         <v>5</v>
       </c>
@@ -15506,7 +15827,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="299" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>58</v>
+      </c>
       <c r="B299">
         <v>5</v>
       </c>
@@ -15547,7 +15871,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="300" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>58</v>
+      </c>
       <c r="B300">
         <v>5</v>
       </c>
@@ -15588,7 +15915,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="301" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>58</v>
+      </c>
       <c r="B301">
         <v>5</v>
       </c>
@@ -15629,7 +15959,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="302" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>58</v>
+      </c>
       <c r="B302">
         <v>5</v>
       </c>
@@ -15670,7 +16003,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="303" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>58</v>
+      </c>
       <c r="B303">
         <v>5</v>
       </c>
@@ -15711,7 +16047,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="304" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>58</v>
+      </c>
       <c r="B304">
         <v>5</v>
       </c>
@@ -15752,7 +16091,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="305" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>58</v>
+      </c>
       <c r="B305">
         <v>5</v>
       </c>
@@ -15793,7 +16135,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="306" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>58</v>
+      </c>
       <c r="B306">
         <v>5</v>
       </c>
@@ -15834,7 +16179,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="307" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>58</v>
+      </c>
       <c r="B307">
         <v>5</v>
       </c>
@@ -15875,7 +16223,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="308" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>58</v>
+      </c>
       <c r="B308">
         <v>5</v>
       </c>
@@ -15916,7 +16267,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="309" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>58</v>
+      </c>
       <c r="B309">
         <v>5</v>
       </c>
@@ -15957,7 +16311,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="310" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>58</v>
+      </c>
       <c r="B310">
         <v>5</v>
       </c>
@@ -15998,7 +16355,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="311" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>58</v>
+      </c>
       <c r="B311">
         <v>5</v>
       </c>
@@ -16039,7 +16399,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="312" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>58</v>
+      </c>
       <c r="B312">
         <v>5</v>
       </c>
@@ -16080,7 +16443,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="313" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>58</v>
+      </c>
       <c r="B313">
         <v>5</v>
       </c>
@@ -16121,7 +16487,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="314" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>58</v>
+      </c>
       <c r="B314">
         <v>5</v>
       </c>
@@ -16162,7 +16531,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="315" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>58</v>
+      </c>
       <c r="B315">
         <v>5</v>
       </c>
@@ -16203,7 +16575,10 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="316" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>58</v>
+      </c>
       <c r="B316">
         <v>5</v>
       </c>
@@ -16245,22 +16620,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O316" xr:uid="{F72756BF-CD78-408E-A5EF-B14FB130BBE6}"/>
+  <autoFilter ref="A1:O316" xr:uid="{F72756BF-CD78-408E-A5EF-B14FB130BBE6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O316">
+      <sortCondition ref="A38"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B1636FD24704A1439BC275B3C3F1C9C6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="96691d2a4c347ae1a5dfc0cee8216ec1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d137487-0b15-4ad9-abee-bf6b36a5a6e0" xmlns:ns3="81cf108f-c583-47b3-8493-b6de3c823d22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f18913b399a1948fbd1deaf24005938" ns2:_="" ns3:_="">
     <xsd:import namespace="3d137487-0b15-4ad9-abee-bf6b36a5a6e0"/>
@@ -16483,6 +16853,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -16492,14 +16871,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF25865C-4B7B-43E6-8BD0-484DAD548BEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87CEC647-6C23-41C1-AD0E-2484640C21F7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16518,6 +16889,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF25865C-4B7B-43E6-8BD0-484DAD548BEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8323A25-8A55-456C-8D2B-5CE95ED6198F}">
   <ds:schemaRefs>

</xml_diff>